<commit_message>
Menu ACT en Mongo para la subida desde ABM
</commit_message>
<xml_diff>
--- a/data/menu.xlsx
+++ b/data/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\Desktop\AG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D3C8BA-50D8-46E9-9552-829FDB4D1B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F0F5A4-EB0E-4371-B481-2F3690F0715A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D1BAB39-A691-44F7-9D9A-87FFC7B3C31C}"/>
   </bookViews>
@@ -227,21 +227,6 @@
     <t>Arroz integral</t>
   </si>
   <si>
-    <t>Pata y muslo con ensalada</t>
-  </si>
-  <si>
-    <t>Pechuga grille gratinada con puré de papas</t>
-  </si>
-  <si>
-    <t>Canelones mixtos con crema de espinaca</t>
-  </si>
-  <si>
-    <t>Sandwich de milanesa con lechuga y tomate</t>
-  </si>
-  <si>
-    <t>Sorrentinos con crema de Roquefort y jamón</t>
-  </si>
-  <si>
     <t>Repollo Colorado</t>
   </si>
   <si>
@@ -267,13 +252,29 @@
   </si>
   <si>
     <t>Cherry con oliva</t>
+  </si>
+  <si>
+    <t>Filet de Merluza con pure mixto</t>
+  </si>
+  <si>
+    <t>Guiso de lentejas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandwich primavera en pan multicereal
+</t>
+  </si>
+  <si>
+    <t>Ravioles Piamontés con salsa 4 quesos</t>
+  </si>
+  <si>
+    <t>Sorrentinos veganos de berenjenas y quinoa con salsa rosa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +289,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -310,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -318,6 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678D72DC-7BA5-41B7-A2F7-6A298D83E786}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,9 +694,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -712,9 +720,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -738,9 +746,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -766,7 +774,7 @@
     </row>
     <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>29</v>
@@ -788,9 +796,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -912,50 +920,51 @@
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="H12" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="H13" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="H14" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H15" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H16" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H17" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H18" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H19" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="8:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="H20" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
envio masivo de mail a la hora de actualizar el menu
</commit_message>
<xml_diff>
--- a/data/menu.xlsx
+++ b/data/menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santi\Desktop\AG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F0F5A4-EB0E-4371-B481-2F3690F0715A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F63CBE6-C4E8-4FC2-BA98-4F102705D956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D1BAB39-A691-44F7-9D9A-87FFC7B3C31C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>menuDelDia</t>
   </si>
@@ -254,20 +254,13 @@
     <t>Cherry con oliva</t>
   </si>
   <si>
-    <t>Filet de Merluza con pure mixto</t>
-  </si>
-  <si>
-    <t>Guiso de lentejas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandwich primavera en pan multicereal
-</t>
-  </si>
-  <si>
-    <t>Ravioles Piamontés con salsa 4 quesos</t>
-  </si>
-  <si>
-    <t>Sorrentinos veganos de berenjenas y quinoa con salsa rosa</t>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>Como</t>
+  </si>
+  <si>
+    <t>Estas</t>
   </si>
 </sst>
 </file>
@@ -663,7 +656,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +714,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -746,8 +739,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -773,9 +766,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
@@ -796,10 +787,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>76</v>
-      </c>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
@@ -843,7 +832,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>

</xml_diff>